<commit_message>
rename pdfs, edit excel
</commit_message>
<xml_diff>
--- a/op-amp-design-calculator-1b.xlsx
+++ b/op-amp-design-calculator-1b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Documents Rick\EE fun\Op Amp Discovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C30EF51-A3C3-453C-8D2A-5EB35BF2FF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F375176-8283-4CF9-9CC3-7EB719E9A134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="327">
   <si>
     <t>R1</t>
   </si>
@@ -1258,6 +1258,9 @@
   </si>
   <si>
     <t>T_lo</t>
+  </si>
+  <si>
+    <t>Vo/Vs</t>
   </si>
 </sst>
 </file>
@@ -3318,22 +3321,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>33130</xdr:colOff>
+      <xdr:colOff>18143</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>11044</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>579782</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>292661</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>149645</xdr:rowOff>
+      <xdr:rowOff>117929</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9E0D4D-E6EF-1C47-A426-516BE8DC127D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{893D1074-5B3F-A340-361A-2224EB7BBFB4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3349,8 +3352,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="883478" y="795131"/>
-          <a:ext cx="1833217" cy="1778557"/>
+          <a:off x="870857" y="843643"/>
+          <a:ext cx="2796375" cy="1687286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4961,8 +4964,8 @@
       <xdr:rowOff>9949</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1794227" cy="549243"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -5155,7 +5158,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -7855,7 +7858,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9780,10 +9783,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9352F31C-6C25-4AEE-91FB-007F3CDD26DC}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9794,177 +9797,177 @@
     <col min="4" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="D2" s="9"/>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D3" s="14"/>
       <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E15"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="F16"/>
+      <c r="E16"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="27">
-        <v>10000</v>
+        <v>83</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.5</v>
       </c>
       <c r="F17"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="27">
+        <v>10000</v>
+      </c>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B19" s="27">
         <v>20000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="18">
-        <f>(B18+B17)/B17</f>
-        <v>3</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E21"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="18">
+        <f>(B19+B18)/B18</f>
+        <v>3</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="6">
-        <f>B16*B21</f>
+      <c r="B23" s="6">
+        <f>B17*B22</f>
         <v>1.5</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E25"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B26" s="18">
-        <v>1</v>
-      </c>
-      <c r="F26"/>
+      <c r="E26"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B27" s="18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F27"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="18">
+        <v>10</v>
+      </c>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B29" s="27">
         <v>1000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="18">
-        <f>B27/B26</f>
-        <v>10</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="18">
+        <f>B28/B27</f>
+        <v>10</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="27">
-        <f>B28*(B29-1)</f>
+      <c r="B31" s="27">
+        <f>B29*(B30-1)</f>
         <v>9000</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>